<commit_message>
fev 2019 (gpm-test =>gpm)
</commit_message>
<xml_diff>
--- a/templates/Invoice.xlsx
+++ b/templates/Invoice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GPM-TEST\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gpm\www\GPM-TEST\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4820B38-15F7-4669-975D-E44FB951B2C8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3A6D6A-8ABE-4C17-B12B-F8513D6B4563}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="9195" windowHeight="5460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">InvoiceFR!$A$1:$G$54</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">InvoiceUSA!$A$1:$G$54</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -1157,7 +1157,7 @@
   <dimension ref="A1:K183"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I9" sqref="I8:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1170,7 +1170,7 @@
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="3"/>
-    <col min="9" max="10" width="11.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" style="63"/>
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
@@ -1249,8 +1249,8 @@
         <v>0</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="I8" s="52" t="s">
-        <v>48</v>
+      <c r="I8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="J8" s="52" t="s">
         <v>49</v>
@@ -1297,7 +1297,9 @@
       <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -2919,7 +2921,7 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.78740157480314965" header="0.11811023622047245" footer="0.31496062992125984"/>
+  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.59055118110236204" bottom="0.78740157480314998" header="0.118110236220472" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter xml:space="preserve">&amp;C&amp;"Times New Roman,Normal"&amp;8&amp;K04-024METCUT RECHERCHES SAS

</xml_diff>